<commit_message>
Se crea repositorio y api para leer los numeros de carga registrados en los monitoreos. Se actualiza encabezado de plantilla de AcumuladosResultados. Se ajusta metodo para descarga de excel con los parametros en horizontal. Se ajusta pantalla de formato-resultado. Ajuste en tamaño de pantalla de acumulacion-resultados., inical de reglas, reglas a validar y el resumen de reglas.
</commit_message>
<xml_diff>
--- a/WebAPI/wwwroot/Plantillas/AcumulacionResultados.xlsx
+++ b/WebAPI/wwwroot/Plantillas/AcumulacionResultados.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nrojast\Documents\Plantillas_cu6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nayeli Rojas\Documents\SICA_INFOTEC\WebAPI\wwwroot\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="4296"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="4290"/>
   </bookViews>
   <sheets>
     <sheet name="Acumulacion Resultados" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>Clave Única</t>
   </si>
   <si>
-    <t>Zona Estratégica</t>
-  </si>
-  <si>
     <t>Laboratorio Realizó Muestreo</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Parámetro</t>
+  </si>
+  <si>
+    <t>Tipo Sitio</t>
   </si>
 </sst>
 </file>
@@ -454,38 +454,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -511,7 +513,7 @@
         <v>13</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>2</v>
@@ -523,22 +525,22 @@
         <v>3</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Pantalla Acumulación de resultados. Corrección en descarga excel.
</commit_message>
<xml_diff>
--- a/WebAPI/wwwroot/Plantillas/AcumulacionResultados.xlsx
+++ b/WebAPI/wwwroot/Plantillas/AcumulacionResultados.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nayeli Rojas\Documents\SICA_INFOTEC\WebAPI\wwwroot\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CONAGUA\GitLab\sica\WebAPI\wwwroot\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2658D25-FFB4-49E7-9FC7-A0609FF0B11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="4290"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acumulacion Resultados" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Clave Muestreo</t>
   </si>
@@ -102,12 +103,21 @@
   </si>
   <si>
     <t>Tipo Sitio</t>
+  </si>
+  <si>
+    <t>Número de Carga</t>
+  </si>
+  <si>
+    <t>Validación por Supervisión</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,13 +167,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -451,120 +461,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>